<commit_message>
Move from CSV to XLSX is complete.
Still need to add summary table for premanifest and then start on final
manifest processing.
</commit_message>
<xml_diff>
--- a/crcManifestProcessorConfig.xlsx
+++ b/crcManifestProcessorConfig.xlsx
@@ -11,12 +11,12 @@
     <sheet name="locationAlias" sheetId="2" r:id="rId2"/>
     <sheet name="priorityMOS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="392">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1189,13 +1189,16 @@
   </si>
   <si>
     <t>O5A</t>
+  </si>
+  <si>
+    <t>JALALALBAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1327,6 +1330,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1629,7 +1639,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1672,11 +1682,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1714,6 +1726,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -2013,7 +2026,7 @@
   <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4186,10 +4199,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4415,16 +4428,16 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>228</v>
+      <c r="A28" s="1" t="s">
+        <v>391</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
@@ -4432,15 +4445,15 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
         <v>151</v>
@@ -4448,15 +4461,15 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
@@ -4464,7 +4477,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
@@ -4472,7 +4485,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
@@ -4480,15 +4493,15 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="B37" t="s">
         <v>91</v>
@@ -4496,7 +4509,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
         <v>91</v>
@@ -4504,7 +4517,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B39" t="s">
         <v>91</v>
@@ -4512,31 +4525,31 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B43" t="s">
         <v>99</v>
@@ -4544,23 +4557,23 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" t="s">
         <v>103</v>
@@ -4568,7 +4581,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B47" t="s">
         <v>103</v>
@@ -4576,15 +4589,15 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B49" t="s">
         <v>104</v>
@@ -4592,7 +4605,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B50" t="s">
         <v>104</v>
@@ -4600,7 +4613,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B51" t="s">
         <v>104</v>
@@ -4608,15 +4621,15 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="B52" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>252</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
         <v>251</v>
@@ -4624,15 +4637,15 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B55" t="s">
         <v>110</v>
@@ -4640,23 +4653,23 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B58" t="s">
         <v>91</v>
@@ -4664,23 +4677,23 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>257</v>
       </c>
       <c r="B59" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>258</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
         <v>138</v>
@@ -4688,15 +4701,15 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B63" t="s">
         <v>137</v>
@@ -4704,7 +4717,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B64" t="s">
         <v>137</v>
@@ -4712,7 +4725,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B65" t="s">
         <v>137</v>
@@ -4720,15 +4733,15 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B67" t="s">
         <v>138</v>
@@ -4736,53 +4749,64 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B70" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B72" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>271</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B74">
+    <sortCondition ref="A2:A74"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated build.xml for distro; add launcher scripts
Updated the Ant build.xml to include the Apache POI dependencies.
Also created some launcher scripts
</commit_message>
<xml_diff>
--- a/crcManifestProcessorConfig.xlsx
+++ b/crcManifestProcessorConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895"/>
   </bookViews>
   <sheets>
     <sheet name="destinationHubMapping" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="396">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1192,13 +1192,25 @@
   </si>
   <si>
     <t>JALALALBAD</t>
+  </si>
+  <si>
+    <t>FENTY</t>
+  </si>
+  <si>
+    <t>PARWAN</t>
+  </si>
+  <si>
+    <t>ZURMAT</t>
+  </si>
+  <si>
+    <t>SELERNO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1340,6 +1352,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1684,9 +1702,12 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2023,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2049,128 +2070,128 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -2181,10 +2202,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -2192,10 +2213,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -2203,7 +2224,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -2214,7 +2235,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -2225,10 +2246,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -2236,10 +2257,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -2247,10 +2268,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -2258,10 +2279,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2269,7 +2290,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -2280,10 +2301,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -2291,10 +2312,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -2302,10 +2323,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -2313,10 +2334,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -2324,7 +2345,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
@@ -2335,7 +2356,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
@@ -2346,10 +2367,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -2357,7 +2378,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
@@ -2368,10 +2389,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -2379,10 +2400,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -2390,7 +2411,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -2401,10 +2422,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -2412,10 +2433,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -2423,10 +2444,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
@@ -2434,7 +2455,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
         <v>16</v>
@@ -2445,21 +2466,21 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>44</v>
+      <c r="A39" s="2" t="s">
+        <v>392</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -2467,10 +2488,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -2478,7 +2499,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
@@ -2489,10 +2510,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
@@ -2500,7 +2521,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
@@ -2511,10 +2532,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -2522,10 +2543,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -2533,7 +2554,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -2544,10 +2565,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -2555,10 +2576,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -2566,7 +2587,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
         <v>23</v>
@@ -2577,10 +2598,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -2588,10 +2609,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -2599,10 +2620,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s">
         <v>17</v>
@@ -2610,7 +2631,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
         <v>23</v>
@@ -2621,10 +2642,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -2632,10 +2653,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
@@ -2643,10 +2664,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
         <v>17</v>
@@ -2654,7 +2675,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>28</v>
@@ -2665,7 +2686,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>28</v>
@@ -2676,7 +2697,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
         <v>23</v>
@@ -2687,7 +2708,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
         <v>28</v>
@@ -2698,10 +2719,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
@@ -2709,10 +2730,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
         <v>17</v>
@@ -2720,7 +2741,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
         <v>23</v>
@@ -2731,10 +2752,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>17</v>
@@ -2742,7 +2763,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
         <v>23</v>
@@ -2753,10 +2774,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -2764,10 +2785,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -2775,7 +2796,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
         <v>28</v>
@@ -2786,10 +2807,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
@@ -2797,10 +2818,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
         <v>17</v>
@@ -2808,7 +2829,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="B71" t="s">
         <v>23</v>
@@ -2819,10 +2840,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C72" t="s">
         <v>17</v>
@@ -2830,10 +2851,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
@@ -2841,10 +2862,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C74" t="s">
         <v>17</v>
@@ -2852,10 +2873,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C75" t="s">
         <v>17</v>
@@ -2863,10 +2884,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
         <v>17</v>
@@ -2874,10 +2895,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
@@ -2885,10 +2906,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C78" t="s">
         <v>17</v>
@@ -2896,7 +2917,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -2907,10 +2928,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
         <v>17</v>
@@ -2918,7 +2939,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
@@ -2929,10 +2950,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C82" t="s">
         <v>17</v>
@@ -2940,10 +2961,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
         <v>17</v>
@@ -2951,10 +2972,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C84" t="s">
         <v>17</v>
@@ -2962,7 +2983,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B85" t="s">
         <v>23</v>
@@ -2973,10 +2994,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B86" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
@@ -2984,10 +3005,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
@@ -2995,10 +3016,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B88" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
         <v>17</v>
@@ -3006,10 +3027,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -3017,10 +3038,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C90" t="s">
         <v>17</v>
@@ -3028,10 +3049,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
@@ -3039,7 +3060,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B92" t="s">
         <v>23</v>
@@ -3050,10 +3071,10 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B93" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
         <v>17</v>
@@ -3061,10 +3082,10 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B94" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C94" t="s">
         <v>17</v>
@@ -3072,7 +3093,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B95" t="s">
         <v>23</v>
@@ -3083,7 +3104,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B96" t="s">
         <v>23</v>
@@ -3094,10 +3115,10 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B97" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C97" t="s">
         <v>17</v>
@@ -3105,7 +3126,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s">
         <v>23</v>
@@ -3116,7 +3137,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B99" t="s">
         <v>16</v>
@@ -3127,10 +3148,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B100" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C100" t="s">
         <v>17</v>
@@ -3138,7 +3159,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B101" t="s">
         <v>16</v>
@@ -3149,7 +3170,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
@@ -3160,10 +3181,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B103" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C103" t="s">
         <v>17</v>
@@ -3171,10 +3192,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B104" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C104" t="s">
         <v>17</v>
@@ -3182,10 +3203,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B105" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C105" t="s">
         <v>17</v>
@@ -3193,21 +3214,21 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B106" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C106" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>110</v>
+      <c r="A107" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="B107" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C107" t="s">
         <v>17</v>
@@ -3215,7 +3236,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B108" t="s">
         <v>23</v>
@@ -3226,10 +3247,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C109" t="s">
         <v>17</v>
@@ -3237,10 +3258,10 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C110" t="s">
         <v>17</v>
@@ -3248,10 +3269,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C111" t="s">
         <v>17</v>
@@ -3259,7 +3280,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B112" t="s">
         <v>23</v>
@@ -3270,7 +3291,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B113" t="s">
         <v>16</v>
@@ -3281,7 +3302,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B114" t="s">
         <v>23</v>
@@ -3292,10 +3313,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B115" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
         <v>17</v>
@@ -3303,10 +3324,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B116" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C116" t="s">
         <v>17</v>
@@ -3314,7 +3335,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B117" t="s">
         <v>23</v>
@@ -3325,10 +3346,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B118" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C118" t="s">
         <v>17</v>
@@ -3336,10 +3357,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B119" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C119" t="s">
         <v>17</v>
@@ -3347,10 +3368,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B120" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C120" t="s">
         <v>17</v>
@@ -3358,10 +3379,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C121" t="s">
         <v>17</v>
@@ -3369,10 +3390,10 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C122" t="s">
         <v>17</v>
@@ -3380,7 +3401,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B123" t="s">
         <v>23</v>
@@ -3391,7 +3412,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B124" t="s">
         <v>23</v>
@@ -3402,10 +3423,10 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B125" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C125" t="s">
         <v>17</v>
@@ -3413,10 +3434,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C126" t="s">
         <v>17</v>
@@ -3424,7 +3445,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s">
         <v>23</v>
@@ -3435,10 +3456,10 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C128" t="s">
         <v>17</v>
@@ -3446,10 +3467,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C129" t="s">
         <v>17</v>
@@ -3457,10 +3478,10 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B130" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C130" t="s">
         <v>17</v>
@@ -3468,10 +3489,10 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B131" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C131" t="s">
         <v>17</v>
@@ -3479,7 +3500,7 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B132" t="s">
         <v>23</v>
@@ -3490,10 +3511,10 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B133" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C133" t="s">
         <v>17</v>
@@ -3501,10 +3522,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B134" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C134" t="s">
         <v>17</v>
@@ -3512,10 +3533,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B135" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C135" t="s">
         <v>17</v>
@@ -3523,7 +3544,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B136" t="s">
         <v>23</v>
@@ -3534,10 +3555,10 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B137" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C137" t="s">
         <v>17</v>
@@ -3545,10 +3566,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B138" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C138" t="s">
         <v>17</v>
@@ -3556,10 +3577,10 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B139" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C139" t="s">
         <v>17</v>
@@ -3567,10 +3588,10 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B140" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C140" t="s">
         <v>17</v>
@@ -3578,7 +3599,7 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B141" t="s">
         <v>23</v>
@@ -3589,10 +3610,10 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B142" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C142" t="s">
         <v>17</v>
@@ -3600,10 +3621,10 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B143" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C143" t="s">
         <v>17</v>
@@ -3611,7 +3632,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B144" t="s">
         <v>28</v>
@@ -3622,10 +3643,10 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B145" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C145" t="s">
         <v>17</v>
@@ -3633,7 +3654,7 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B146" t="s">
         <v>23</v>
@@ -3644,7 +3665,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B147" t="s">
         <v>23</v>
@@ -3655,10 +3676,10 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B148" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C148" t="s">
         <v>17</v>
@@ -3666,10 +3687,10 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B149" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C149" t="s">
         <v>17</v>
@@ -3677,7 +3698,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B150" t="s">
         <v>23</v>
@@ -3688,10 +3709,10 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B151" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C151" t="s">
         <v>17</v>
@@ -3699,10 +3720,10 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B152" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C152" t="s">
         <v>17</v>
@@ -3710,7 +3731,7 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B153" t="s">
         <v>28</v>
@@ -3721,10 +3742,10 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C154" t="s">
         <v>17</v>
@@ -3732,10 +3753,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B155" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C155" t="s">
         <v>17</v>
@@ -3743,10 +3764,10 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B156" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C156" t="s">
         <v>17</v>
@@ -3754,21 +3775,21 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B157" t="s">
+        <v>16</v>
+      </c>
+      <c r="C157" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B158" t="s">
         <v>28</v>
-      </c>
-      <c r="C157" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158" t="s">
-        <v>161</v>
-      </c>
-      <c r="B158" t="s">
-        <v>16</v>
       </c>
       <c r="C158" t="s">
         <v>17</v>
@@ -3776,98 +3797,98 @@
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B159" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="C159" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>174</v>
       </c>
       <c r="C160" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B161" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="C161" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B162" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="C162" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B163" t="s">
-        <v>23</v>
+        <v>176</v>
       </c>
       <c r="C163" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B164" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="C164" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B165" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="C165" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="C166" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B167" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C167" t="s">
         <v>172</v>
@@ -3875,10 +3896,10 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C168" t="s">
         <v>172</v>
@@ -3886,7 +3907,7 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B169" t="s">
         <v>176</v>
@@ -3897,10 +3918,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B170" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C170" t="s">
         <v>172</v>
@@ -3908,7 +3929,7 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B171" t="s">
         <v>176</v>
@@ -3919,10 +3940,10 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B172" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C172" t="s">
         <v>172</v>
@@ -3930,7 +3951,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B173" t="s">
         <v>176</v>
@@ -3941,10 +3962,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B174" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C174" t="s">
         <v>172</v>
@@ -3952,7 +3973,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
         <v>176</v>
@@ -3963,7 +3984,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B176" t="s">
         <v>176</v>
@@ -3974,10 +3995,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B177" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C177" t="s">
         <v>172</v>
@@ -3985,10 +4006,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B178" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C178" t="s">
         <v>172</v>
@@ -3996,10 +4017,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B179" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C179" t="s">
         <v>172</v>
@@ -4007,10 +4028,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B180" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C180" t="s">
         <v>172</v>
@@ -4018,10 +4039,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B181" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C181" t="s">
         <v>172</v>
@@ -4029,10 +4050,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B182" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C182" t="s">
         <v>172</v>
@@ -4040,7 +4061,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B183" t="s">
         <v>176</v>
@@ -4051,7 +4072,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>190</v>
+        <v>13</v>
       </c>
       <c r="B184" t="s">
         <v>176</v>
@@ -4062,10 +4083,10 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B185" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C185" t="s">
         <v>172</v>
@@ -4073,7 +4094,7 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B186" t="s">
         <v>176</v>
@@ -4084,125 +4105,162 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>193</v>
+        <v>3</v>
       </c>
       <c r="B187" t="s">
-        <v>174</v>
+        <v>3</v>
       </c>
       <c r="C187" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="B188" t="s">
-        <v>171</v>
+        <v>3</v>
       </c>
       <c r="C188" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>194</v>
+        <v>6</v>
       </c>
       <c r="B189" t="s">
-        <v>179</v>
+        <v>3</v>
       </c>
       <c r="C189" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>7</v>
       </c>
       <c r="B190" t="s">
-        <v>176</v>
+        <v>3</v>
       </c>
       <c r="C190" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>196</v>
+        <v>8</v>
       </c>
       <c r="B191" t="s">
-        <v>176</v>
+        <v>3</v>
       </c>
       <c r="C191" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B192" t="s">
-        <v>176</v>
+        <v>3</v>
       </c>
       <c r="C192" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
       <c r="B193" t="s">
-        <v>174</v>
+        <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>198</v>
+        <v>11</v>
       </c>
       <c r="B194" t="s">
-        <v>176</v>
+        <v>3</v>
       </c>
       <c r="C194" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>199</v>
+        <v>12</v>
       </c>
       <c r="B195" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="C195" t="s">
-        <v>200</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
+        <v>13</v>
+      </c>
+      <c r="B196" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>14</v>
+      </c>
+      <c r="B197" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>199</v>
+      </c>
+      <c r="B198" t="s">
+        <v>199</v>
+      </c>
+      <c r="C198" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
         <v>201</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B199" t="s">
         <v>199</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C199" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C199">
+    <sortCondition ref="C2:C199"/>
+    <sortCondition ref="A2:A199"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4757,55 +4815,71 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>266</v>
+        <v>395</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B72" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
+        <v>270</v>
+      </c>
+      <c r="B74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
         <v>271</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>167</v>
       </c>
     </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>394</v>
+      </c>
+      <c r="B76" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B74">
-    <sortCondition ref="A2:A74"/>
+  <sortState ref="A2:B76">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4815,7 +4889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>